<commit_message>
add menu update data
</commit_message>
<xml_diff>
--- a/data/Direktori_SBR_20260114.xlsx
+++ b/data/Direktori_SBR_20260114.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\otomatisasidirgc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6EF7A3-7AE5-4795-AEDB-E2CB9206E80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F215BD-B157-432B-9903-76B77CCACBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>idsbr</t>
   </si>
@@ -44,12 +44,6 @@
 4:ganda</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>PENGGILINGAN PADI KATIRAN</t>
   </si>
   <si>
@@ -57,15 +51,61 @@
   </si>
   <si>
     <t>JL. BALAI</t>
+  </si>
+  <si>
+    <t>PENGGILINGAN PADI IBERAHIM</t>
+  </si>
+  <si>
+    <t>PENGGILINGAN PADI LERANG USAT</t>
+  </si>
+  <si>
+    <t>PENGGILINGAN PADI SULING LIHIU</t>
+  </si>
+  <si>
+    <t>PENGGILINGAN PADI LEWI USAT</t>
+  </si>
+  <si>
+    <t>PENGGILINGAN PADI LIAN NCAU</t>
+  </si>
+  <si>
+    <t>PENGGILINGAN PADI USAT JALUNG</t>
+  </si>
+  <si>
+    <t>PENGGILINGAN PADI NASRUN</t>
+  </si>
+  <si>
+    <t>JL. NIAGA MAKBANG PEMBOH</t>
+  </si>
+  <si>
+    <t>JL. NIAGA PAMONG TAWAI</t>
+  </si>
+  <si>
+    <t>JL. PINER, RT. 012, LONG BELUAH</t>
+  </si>
+  <si>
+    <t>RT. 002</t>
+  </si>
+  <si>
+    <t>RT. 004</t>
+  </si>
+  <si>
+    <t>JL. LINGAI, RT. 03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -85,6 +125,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -94,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,20 +148,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{34353540-8870-44CF-AF08-A1BA8CC8C0A2}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{04215CA9-4A4D-401D-B859-234D6296DE7E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -452,15 +521,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,62 +552,190 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
+        <v>6868001</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2.8413431</v>
+      </c>
+      <c r="E2" s="4">
+        <v>117.3725165</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>6868008</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2.8413484000000002</v>
+      </c>
+      <c r="E3" s="4">
+        <v>117.3725335</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>6868017</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.8413412999999998</v>
+      </c>
+      <c r="E4" s="4">
+        <v>117.37251670000001</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>6868030</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.8413506000000002</v>
+      </c>
+      <c r="E5" s="4">
+        <v>117.3725146</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>6868042</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.8413447999999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>117.3725242</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6868057</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2.8413512999999999</v>
+      </c>
+      <c r="E7" s="4">
+        <v>117.37251620000001</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>6868070</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.8413461999999998</v>
+      </c>
+      <c r="E8" s="4">
+        <v>117.3725197</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>6868082</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="D9" s="4">
         <v>2.8413403000000002</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E9" s="4">
         <v>117.3725153</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>6868100</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4">
         <v>2.8413395000000001</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E10" s="4">
         <v>117.3725156</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3"/>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1 A4:F4 F2:F3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>